<commit_message>
Applied code improvements: enhanced error handling, type safety, and configurability
</commit_message>
<xml_diff>
--- a/outputs/validation_report.xlsx
+++ b/outputs/validation_report.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summary" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Validation" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,17 +17,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
-      <sz val="14"/>
     </font>
   </fonts>
   <fills count="2">
@@ -50,9 +46,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -418,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -427,42 +422,35 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
-          <t>USB PD Validation Report</t>
+          <t>Metric</t>
         </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>TOC Entries</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>1360</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>TOC Entries</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>1360</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
           <t>Content Items</t>
         </is>
       </c>
-      <c r="B4" t="n">
+      <c r="B3" t="n">
         <v>25760</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Status</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>PASS</t>
-        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>